<commit_message>
timetable with the breaks
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -441,22 +441,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10:00</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>09:30</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>12:00</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>13:00</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -488,42 +488,42 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>DSA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>DSA - Lisa</t>
+          <t>Tea Break</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Computer Networks - Bhavya B G</t>
+          <t>Cryptography</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Lunch Break</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Computer organization - Natesh </t>
+          <t>DBMS</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Python - Henry</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cryptography - Ramakrishna Hegde </t>
+          <t>Computer organization</t>
         </is>
       </c>
     </row>
@@ -535,42 +535,42 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>DSA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>DSA - Lisa</t>
+          <t>Tea Break</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Computer Networks - Bhavya B G</t>
+          <t>Cryptography</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Lunch Break</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Computer organization - Natesh </t>
+          <t>DBMS</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Python - Henry</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cryptography - Ramakrishna Hegde </t>
+          <t>Computer organization</t>
         </is>
       </c>
     </row>
@@ -582,42 +582,42 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>DSA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>DSA - Lisa</t>
+          <t>Tea Break</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Computer Networks - Bhavya B G</t>
+          <t>Cryptography</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Lunch Break</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Computer organization - Natesh </t>
+          <t>DBMS</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Python - Henry</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cryptography - Ramakrishna Hegde </t>
+          <t>Computer organization</t>
         </is>
       </c>
     </row>
@@ -629,42 +629,42 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>DSA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>DSA - Lisa</t>
+          <t>Tea Break</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Computer Networks - Bhavya B G</t>
+          <t>Cryptography</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Lunch Break</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Computer organization - Natesh </t>
+          <t>DBMS</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Python - Henry</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cryptography - Ramakrishna Hegde </t>
+          <t>Computer organization</t>
         </is>
       </c>
     </row>
@@ -676,42 +676,42 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>DSA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>DSA - Lisa</t>
+          <t>Tea Break</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Computer Networks - Bhavya B G</t>
+          <t>Cryptography</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Lunch Break</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Computer organization - Natesh </t>
+          <t>DBMS</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Python - Henry</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cryptography - Ramakrishna Hegde </t>
+          <t>Computer organization</t>
         </is>
       </c>
     </row>
@@ -723,42 +723,42 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>DSA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>DBMS - Chaitra N C</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DSA - Lisa</t>
+          <t>Tea Break</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Computer Networks - Bhavya B G</t>
+          <t>Cryptography</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Lunch Break</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Computer organization - Natesh </t>
+          <t>DBMS</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Python - Henry</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cryptography - Ramakrishna Hegde </t>
+          <t>Computer organization</t>
         </is>
       </c>
     </row>

</xml_diff>